<commit_message>
Update cpp and python for Kmeans
</commit_message>
<xml_diff>
--- a/data_slopes.xlsx
+++ b/data_slopes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lilia\github\Projet_ter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20B7C079-69C9-4D08-924F-E17CE982DEA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B6DC603-98C7-4D00-9963-8B7E784B8772}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="282">
   <si>
     <t>p1</t>
   </si>
@@ -34,12 +34,120 @@
     <t>classe</t>
   </si>
   <si>
+    <t>-0.382433</t>
+  </si>
+  <si>
+    <t>0.24</t>
+  </si>
+  <si>
+    <t>-0.464121</t>
+  </si>
+  <si>
+    <t>0.26</t>
+  </si>
+  <si>
+    <t>-0.157545</t>
+  </si>
+  <si>
+    <t>-1.00392</t>
+  </si>
+  <si>
+    <t>0.44</t>
+  </si>
+  <si>
+    <t>-0.874338</t>
+  </si>
+  <si>
+    <t>0.27</t>
+  </si>
+  <si>
+    <t>-0.58666</t>
+  </si>
+  <si>
+    <t>0.29</t>
+  </si>
+  <si>
+    <t>-0.696073</t>
+  </si>
+  <si>
+    <t>0.42</t>
+  </si>
+  <si>
+    <t>-0.883361</t>
+  </si>
+  <si>
+    <t>0.38</t>
+  </si>
+  <si>
+    <t>-0.596812</t>
+  </si>
+  <si>
+    <t>0.33</t>
+  </si>
+  <si>
+    <t>-0.710611</t>
+  </si>
+  <si>
+    <t>0.08</t>
+  </si>
+  <si>
+    <t>-0.552036</t>
+  </si>
+  <si>
+    <t>0.49</t>
+  </si>
+  <si>
+    <t>-0.350628</t>
+  </si>
+  <si>
+    <t>0.11</t>
+  </si>
+  <si>
+    <t>-0.640968</t>
+  </si>
+  <si>
+    <t>0.22</t>
+  </si>
+  <si>
     <t>-0.739211</t>
   </si>
   <si>
     <t>0.56</t>
   </si>
   <si>
+    <t>-0.726504</t>
+  </si>
+  <si>
+    <t>-0.421634</t>
+  </si>
+  <si>
+    <t>0.28</t>
+  </si>
+  <si>
+    <t>-0.687725</t>
+  </si>
+  <si>
+    <t>-0.784448</t>
+  </si>
+  <si>
+    <t>0.14</t>
+  </si>
+  <si>
+    <t>-0.572758</t>
+  </si>
+  <si>
+    <t>0.72</t>
+  </si>
+  <si>
+    <t>-0.182305</t>
+  </si>
+  <si>
+    <t>-1.19899</t>
+  </si>
+  <si>
+    <t>0.48</t>
+  </si>
+  <si>
     <t>-0.0772961</t>
   </si>
   <si>
@@ -49,6 +157,9 @@
     <t>1.18</t>
   </si>
   <si>
+    <t>-0.695212</t>
+  </si>
+  <si>
     <t>-0.578238</t>
   </si>
   <si>
@@ -64,6 +175,12 @@
     <t>3.41</t>
   </si>
   <si>
+    <t>-0.672398</t>
+  </si>
+  <si>
+    <t>0.81</t>
+  </si>
+  <si>
     <t>-0.378643</t>
   </si>
   <si>
@@ -73,6 +190,15 @@
     <t>5.19</t>
   </si>
   <si>
+    <t>-0.65659</t>
+  </si>
+  <si>
+    <t>-0.321872</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
     <t>-0.240885</t>
   </si>
   <si>
@@ -91,12 +217,27 @@
     <t>7.62</t>
   </si>
   <si>
+    <t>-0.812343</t>
+  </si>
+  <si>
+    <t>0.19</t>
+  </si>
+  <si>
+    <t>-0.556888</t>
+  </si>
+  <si>
     <t>-0.748325</t>
   </si>
   <si>
     <t>0.88</t>
   </si>
   <si>
+    <t>-0.737077</t>
+  </si>
+  <si>
+    <t>0.51</t>
+  </si>
+  <si>
     <t>-0.775512</t>
   </si>
   <si>
@@ -112,18 +253,81 @@
     <t>2.17</t>
   </si>
   <si>
+    <t>-0.419549</t>
+  </si>
+  <si>
+    <t>-0.753625</t>
+  </si>
+  <si>
+    <t>0.21</t>
+  </si>
+  <si>
+    <t>-0.50997</t>
+  </si>
+  <si>
     <t>-0.728985</t>
   </si>
   <si>
     <t>0.69</t>
   </si>
   <si>
+    <t>-0.623524</t>
+  </si>
+  <si>
+    <t>0.63</t>
+  </si>
+  <si>
+    <t>-0.887724</t>
+  </si>
+  <si>
+    <t>-0.192734</t>
+  </si>
+  <si>
+    <t>-1.26672</t>
+  </si>
+  <si>
+    <t>0.75</t>
+  </si>
+  <si>
     <t>-0.811741</t>
   </si>
   <si>
     <t>1.7</t>
   </si>
   <si>
+    <t>-0.537823</t>
+  </si>
+  <si>
+    <t>0.36</t>
+  </si>
+  <si>
+    <t>-0.380554</t>
+  </si>
+  <si>
+    <t>-1.23258</t>
+  </si>
+  <si>
+    <t>0.89</t>
+  </si>
+  <si>
+    <t>-0.596644</t>
+  </si>
+  <si>
+    <t>-0.484921</t>
+  </si>
+  <si>
+    <t>-0.330655</t>
+  </si>
+  <si>
+    <t>-0.514581</t>
+  </si>
+  <si>
+    <t>-0.809495</t>
+  </si>
+  <si>
+    <t>0.94</t>
+  </si>
+  <si>
     <t>-0.214928</t>
   </si>
   <si>
@@ -139,6 +343,36 @@
     <t>1.11</t>
   </si>
   <si>
+    <t>-0.634177</t>
+  </si>
+  <si>
+    <t>-0.0758436</t>
+  </si>
+  <si>
+    <t>-1.13744</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>-0.186538</t>
+  </si>
+  <si>
+    <t>-0.843318</t>
+  </si>
+  <si>
+    <t>0.87</t>
+  </si>
+  <si>
+    <t>-0.469656</t>
+  </si>
+  <si>
+    <t>-0.653863</t>
+  </si>
+  <si>
+    <t>0.52</t>
+  </si>
+  <si>
     <t>-0.819733</t>
   </si>
   <si>
@@ -166,6 +400,36 @@
     <t>1.17</t>
   </si>
   <si>
+    <t>-0.760372</t>
+  </si>
+  <si>
+    <t>-0.289906</t>
+  </si>
+  <si>
+    <t>-1.21175</t>
+  </si>
+  <si>
+    <t>-0.334773</t>
+  </si>
+  <si>
+    <t>-1.35218</t>
+  </si>
+  <si>
+    <t>0.45</t>
+  </si>
+  <si>
+    <t>-0.44402</t>
+  </si>
+  <si>
+    <t>0.43</t>
+  </si>
+  <si>
+    <t>-0.69583</t>
+  </si>
+  <si>
+    <t>0.37</t>
+  </si>
+  <si>
     <t>-0.222002</t>
   </si>
   <si>
@@ -175,24 +439,90 @@
     <t>1.41</t>
   </si>
   <si>
+    <t>-0.56359</t>
+  </si>
+  <si>
+    <t>-0.946903</t>
+  </si>
+  <si>
+    <t>0.57</t>
+  </si>
+  <si>
+    <t>-0.566631</t>
+  </si>
+  <si>
+    <t>0.79</t>
+  </si>
+  <si>
     <t>-0.0286826</t>
   </si>
   <si>
     <t>-1.16659</t>
   </si>
   <si>
-    <t>0.51</t>
+    <t>-0.714653</t>
+  </si>
+  <si>
+    <t>0.16</t>
+  </si>
+  <si>
+    <t>-0.501932</t>
+  </si>
+  <si>
+    <t>0.15</t>
+  </si>
+  <si>
+    <t>-0.463264</t>
+  </si>
+  <si>
+    <t>-1.23766</t>
+  </si>
+  <si>
+    <t>0.66</t>
+  </si>
+  <si>
+    <t>-0.431173</t>
   </si>
   <si>
     <t>-0.749791</t>
   </si>
   <si>
+    <t>-0.620553</t>
+  </si>
+  <si>
+    <t>-0.907839</t>
+  </si>
+  <si>
+    <t>0.53</t>
+  </si>
+  <si>
+    <t>-0.0946372</t>
+  </si>
+  <si>
+    <t>-0.929416</t>
+  </si>
+  <si>
+    <t>-0.764024</t>
+  </si>
+  <si>
+    <t>-1.848</t>
+  </si>
+  <si>
+    <t>-0.847777</t>
+  </si>
+  <si>
+    <t>0.76</t>
+  </si>
+  <si>
     <t>-0.747629</t>
   </si>
   <si>
     <t>0.84</t>
   </si>
   <si>
+    <t>-0.65788</t>
+  </si>
+  <si>
     <t>-0.510764</t>
   </si>
   <si>
@@ -202,10 +532,169 @@
     <t>0.8</t>
   </si>
   <si>
+    <t>-0.363679</t>
+  </si>
+  <si>
+    <t>-0.792229</t>
+  </si>
+  <si>
+    <t>-0.502713</t>
+  </si>
+  <si>
+    <t>0.31</t>
+  </si>
+  <si>
+    <t>-0.760449</t>
+  </si>
+  <si>
+    <t>-0.548903</t>
+  </si>
+  <si>
+    <t>-0.229085</t>
+  </si>
+  <si>
+    <t>-1.03638</t>
+  </si>
+  <si>
+    <t>0.35</t>
+  </si>
+  <si>
+    <t>-0.470289</t>
+  </si>
+  <si>
+    <t>-0.949183</t>
+  </si>
+  <si>
+    <t>-0.801267</t>
+  </si>
+  <si>
+    <t>0.58</t>
+  </si>
+  <si>
+    <t>-0.831323</t>
+  </si>
+  <si>
+    <t>0.55</t>
+  </si>
+  <si>
+    <t>-0.612363</t>
+  </si>
+  <si>
+    <t>-0.665272</t>
+  </si>
+  <si>
+    <t>0.54</t>
+  </si>
+  <si>
+    <t>-0.590847</t>
+  </si>
+  <si>
+    <t>-0.52863</t>
+  </si>
+  <si>
+    <t>-0.887125</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>-0.606362</t>
+  </si>
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>-0.49464</t>
+  </si>
+  <si>
+    <t>-0.9647</t>
+  </si>
+  <si>
+    <t>0.92</t>
+  </si>
+  <si>
+    <t>-1.0451</t>
+  </si>
+  <si>
+    <t>-0.492966</t>
+  </si>
+  <si>
+    <t>-0.138995</t>
+  </si>
+  <si>
+    <t>-1.18503</t>
+  </si>
+  <si>
+    <t>-0.729717</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>-0.553617</t>
+  </si>
+  <si>
+    <t>0.18</t>
+  </si>
+  <si>
+    <t>-0.396352</t>
+  </si>
+  <si>
+    <t>-1.54727</t>
+  </si>
+  <si>
+    <t>0.06</t>
+  </si>
+  <si>
+    <t>-0.507404</t>
+  </si>
+  <si>
+    <t>-0.459528</t>
+  </si>
+  <si>
+    <t>-0.847214</t>
+  </si>
+  <si>
+    <t>0.47</t>
+  </si>
+  <si>
+    <t>0.03</t>
+  </si>
+  <si>
+    <t>-0.39184</t>
+  </si>
+  <si>
+    <t>-0.963918</t>
+  </si>
+  <si>
+    <t>0.73</t>
+  </si>
+  <si>
+    <t>-0.484104</t>
+  </si>
+  <si>
     <t>-0.796475</t>
   </si>
   <si>
-    <t>0.63</t>
+    <t>-0.804213</t>
+  </si>
+  <si>
+    <t>-0.963243</t>
+  </si>
+  <si>
+    <t>-0.484005</t>
+  </si>
+  <si>
+    <t>0.41</t>
+  </si>
+  <si>
+    <t>-0.607861</t>
+  </si>
+  <si>
+    <t>-0.966325</t>
+  </si>
+  <si>
+    <t>0.07</t>
   </si>
   <si>
     <t>-0.10048</t>
@@ -217,15 +706,33 @@
     <t>1.01</t>
   </si>
   <si>
+    <t>-0.648432</t>
+  </si>
+  <si>
     <t>-0.654327</t>
   </si>
   <si>
     <t>1.1</t>
   </si>
   <si>
+    <t>-0.472126</t>
+  </si>
+  <si>
+    <t>0.13</t>
+  </si>
+  <si>
     <t>-1.01265</t>
   </si>
   <si>
+    <t>-0.844562</t>
+  </si>
+  <si>
+    <t>-0.754092</t>
+  </si>
+  <si>
+    <t>0.32</t>
+  </si>
+  <si>
     <t>-0.0972445</t>
   </si>
   <si>
@@ -235,6 +742,33 @@
     <t>1.16</t>
   </si>
   <si>
+    <t>-0.575801</t>
+  </si>
+  <si>
+    <t>0.34</t>
+  </si>
+  <si>
+    <t>-0.511818</t>
+  </si>
+  <si>
+    <t>-0.662543</t>
+  </si>
+  <si>
+    <t>0.12</t>
+  </si>
+  <si>
+    <t>-0.641963</t>
+  </si>
+  <si>
+    <t>-0.183864</t>
+  </si>
+  <si>
+    <t>-1.05198</t>
+  </si>
+  <si>
+    <t>-0.645043</t>
+  </si>
+  <si>
     <t>-0.29755</t>
   </si>
   <si>
@@ -244,6 +778,39 @@
     <t>1.34</t>
   </si>
   <si>
+    <t>-0.289522</t>
+  </si>
+  <si>
+    <t>-1.25728</t>
+  </si>
+  <si>
+    <t>-0.0421108</t>
+  </si>
+  <si>
+    <t>-0.88621</t>
+  </si>
+  <si>
+    <t>1.02</t>
+  </si>
+  <si>
+    <t>-0.379015</t>
+  </si>
+  <si>
+    <t>-0.914424</t>
+  </si>
+  <si>
+    <t>-0.571283</t>
+  </si>
+  <si>
+    <t>0.62</t>
+  </si>
+  <si>
+    <t>-0.409856</t>
+  </si>
+  <si>
+    <t>-0.489344</t>
+  </si>
+  <si>
     <t>-0.267481</t>
   </si>
   <si>
@@ -253,10 +820,52 @@
     <t>2.71</t>
   </si>
   <si>
+    <t>-0.460627</t>
+  </si>
+  <si>
+    <t>-0.650256</t>
+  </si>
+  <si>
+    <t>-0.122024</t>
+  </si>
+  <si>
+    <t>-0.9469</t>
+  </si>
+  <si>
+    <t>1.22</t>
+  </si>
+  <si>
+    <t>-0.123844</t>
+  </si>
+  <si>
+    <t>-0.814217</t>
+  </si>
+  <si>
+    <t>0.46</t>
+  </si>
+  <si>
     <t>-0.126822</t>
   </si>
   <si>
     <t>-1.5671</t>
+  </si>
+  <si>
+    <t>-0.0150054</t>
+  </si>
+  <si>
+    <t>-0.994464</t>
+  </si>
+  <si>
+    <t>-0.0922679</t>
+  </si>
+  <si>
+    <t>-1.11051</t>
+  </si>
+  <si>
+    <t>-0.101081</t>
+  </si>
+  <si>
+    <t>-1.57052</t>
   </si>
 </sst>
 </file>
@@ -1097,9 +1706,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1136,10 +1745,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1147,7 +1756,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -1164,10 +1773,10 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1175,13 +1784,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1189,13 +1798,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1203,13 +1812,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1217,13 +1826,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1231,13 +1840,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1245,13 +1854,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1259,13 +1868,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1273,13 +1882,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1287,253 +1896,1933 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
+        <v>56</v>
+      </c>
+      <c r="C27" t="s">
+        <v>36</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>77</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>78</v>
       </c>
-      <c r="C31" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31">
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" t="s">
+        <v>88</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" t="s">
+        <v>90</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" t="s">
+        <v>79</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" t="s">
+        <v>101</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" t="s">
+        <v>104</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>105</v>
+      </c>
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" t="s">
+        <v>106</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" t="s">
+        <v>41</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" t="s">
+        <v>109</v>
+      </c>
+      <c r="C55" t="s">
+        <v>110</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>111</v>
+      </c>
+      <c r="B56" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" t="s">
+        <v>113</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>114</v>
+      </c>
+      <c r="B57" t="s">
+        <v>114</v>
+      </c>
+      <c r="C57" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>115</v>
+      </c>
+      <c r="B58" t="s">
+        <v>115</v>
+      </c>
+      <c r="C58" t="s">
+        <v>116</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>117</v>
+      </c>
+      <c r="B59" t="s">
+        <v>118</v>
+      </c>
+      <c r="C59" t="s">
+        <v>119</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>120</v>
+      </c>
+      <c r="B60" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" t="s">
+        <v>122</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>123</v>
+      </c>
+      <c r="B61" t="s">
+        <v>124</v>
+      </c>
+      <c r="C61" t="s">
+        <v>125</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>126</v>
+      </c>
+      <c r="B62" t="s">
+        <v>126</v>
+      </c>
+      <c r="C62" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>127</v>
+      </c>
+      <c r="B63" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63" t="s">
+        <v>20</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>129</v>
+      </c>
+      <c r="B64" t="s">
+        <v>130</v>
+      </c>
+      <c r="C64" t="s">
+        <v>131</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>132</v>
+      </c>
+      <c r="B65" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" t="s">
+        <v>133</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>134</v>
+      </c>
+      <c r="B66" t="s">
+        <v>134</v>
+      </c>
+      <c r="C66" t="s">
+        <v>135</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>136</v>
+      </c>
+      <c r="B67" t="s">
+        <v>137</v>
+      </c>
+      <c r="C67" t="s">
+        <v>138</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>139</v>
+      </c>
+      <c r="B68" t="s">
+        <v>139</v>
+      </c>
+      <c r="C68" t="s">
+        <v>135</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>140</v>
+      </c>
+      <c r="B69" t="s">
+        <v>140</v>
+      </c>
+      <c r="C69" t="s">
+        <v>141</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>142</v>
+      </c>
+      <c r="B70" t="s">
+        <v>142</v>
+      </c>
+      <c r="C70" t="s">
+        <v>143</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>144</v>
+      </c>
+      <c r="B71" t="s">
+        <v>145</v>
+      </c>
+      <c r="C71" t="s">
+        <v>71</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>146</v>
+      </c>
+      <c r="B72" t="s">
+        <v>146</v>
+      </c>
+      <c r="C72" t="s">
+        <v>147</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>148</v>
+      </c>
+      <c r="B73" t="s">
+        <v>148</v>
+      </c>
+      <c r="C73" t="s">
+        <v>149</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>150</v>
+      </c>
+      <c r="B74" t="s">
+        <v>151</v>
+      </c>
+      <c r="C74" t="s">
+        <v>152</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>153</v>
+      </c>
+      <c r="B75" t="s">
+        <v>153</v>
+      </c>
+      <c r="C75" t="s">
+        <v>26</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>154</v>
+      </c>
+      <c r="B76" t="s">
+        <v>154</v>
+      </c>
+      <c r="C76" t="s">
+        <v>125</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>155</v>
+      </c>
+      <c r="B77" t="s">
+        <v>155</v>
+      </c>
+      <c r="C77" t="s">
+        <v>20</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>156</v>
+      </c>
+      <c r="B78" t="s">
+        <v>156</v>
+      </c>
+      <c r="C78" t="s">
+        <v>157</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>158</v>
+      </c>
+      <c r="B79" t="s">
+        <v>159</v>
+      </c>
+      <c r="C79" t="s">
+        <v>152</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>160</v>
+      </c>
+      <c r="B80" t="s">
+        <v>160</v>
+      </c>
+      <c r="C80" t="s">
+        <v>10</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>161</v>
+      </c>
+      <c r="B81" t="s">
+        <v>162</v>
+      </c>
+      <c r="C81" t="s">
+        <v>163</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>164</v>
+      </c>
+      <c r="B82" t="s">
+        <v>164</v>
+      </c>
+      <c r="C82" t="s">
+        <v>165</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>166</v>
+      </c>
+      <c r="B83" t="s">
+        <v>166</v>
+      </c>
+      <c r="C83" t="s">
+        <v>12</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>167</v>
+      </c>
+      <c r="B84" t="s">
+        <v>168</v>
+      </c>
+      <c r="C84" t="s">
+        <v>169</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>170</v>
+      </c>
+      <c r="B85" t="s">
+        <v>170</v>
+      </c>
+      <c r="C85" t="s">
+        <v>5</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>171</v>
+      </c>
+      <c r="B86" t="s">
+        <v>171</v>
+      </c>
+      <c r="C86" t="s">
+        <v>18</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" t="s">
+        <v>172</v>
+      </c>
+      <c r="C87" t="s">
+        <v>173</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" t="s">
+        <v>174</v>
+      </c>
+      <c r="C88" t="s">
+        <v>28</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>175</v>
+      </c>
+      <c r="B89" t="s">
+        <v>175</v>
+      </c>
+      <c r="C89" t="s">
+        <v>173</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>176</v>
+      </c>
+      <c r="B90" t="s">
+        <v>177</v>
+      </c>
+      <c r="C90" t="s">
+        <v>178</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>179</v>
+      </c>
+      <c r="B91" t="s">
+        <v>179</v>
+      </c>
+      <c r="C91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>0</v>
+      </c>
+      <c r="B92" t="s">
+        <v>180</v>
+      </c>
+      <c r="C92" t="s">
+        <v>135</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>181</v>
+      </c>
+      <c r="B93" t="s">
+        <v>181</v>
+      </c>
+      <c r="C93" t="s">
+        <v>182</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>183</v>
+      </c>
+      <c r="B94" t="s">
+        <v>183</v>
+      </c>
+      <c r="C94" t="s">
+        <v>184</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>185</v>
+      </c>
+      <c r="B95" t="s">
+        <v>185</v>
+      </c>
+      <c r="C95" t="s">
+        <v>20</v>
+      </c>
+      <c r="D95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>186</v>
+      </c>
+      <c r="B96" t="s">
+        <v>186</v>
+      </c>
+      <c r="C96" t="s">
+        <v>187</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>188</v>
+      </c>
+      <c r="B97" t="s">
+        <v>188</v>
+      </c>
+      <c r="C97" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>189</v>
+      </c>
+      <c r="B98" t="s">
+        <v>189</v>
+      </c>
+      <c r="C98" t="s">
+        <v>135</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>190</v>
+      </c>
+      <c r="B99" t="s">
+        <v>190</v>
+      </c>
+      <c r="C99" t="s">
+        <v>191</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>192</v>
+      </c>
+      <c r="B100" t="s">
+        <v>192</v>
+      </c>
+      <c r="C100" t="s">
+        <v>193</v>
+      </c>
+      <c r="D100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>194</v>
+      </c>
+      <c r="B101" t="s">
+        <v>194</v>
+      </c>
+      <c r="C101" t="s">
+        <v>92</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>195</v>
+      </c>
+      <c r="B102" t="s">
+        <v>195</v>
+      </c>
+      <c r="C102" t="s">
+        <v>196</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>197</v>
+      </c>
+      <c r="B103" t="s">
+        <v>197</v>
+      </c>
+      <c r="C103" t="s">
+        <v>28</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>198</v>
+      </c>
+      <c r="B104" t="s">
+        <v>198</v>
+      </c>
+      <c r="C104" t="s">
+        <v>10</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>199</v>
+      </c>
+      <c r="B105" t="s">
+        <v>200</v>
+      </c>
+      <c r="C105" t="s">
+        <v>187</v>
+      </c>
+      <c r="D105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>201</v>
+      </c>
+      <c r="B106" t="s">
+        <v>201</v>
+      </c>
+      <c r="C106" t="s">
+        <v>202</v>
+      </c>
+      <c r="D106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>203</v>
+      </c>
+      <c r="B107" t="s">
+        <v>203</v>
+      </c>
+      <c r="C107" t="s">
+        <v>204</v>
+      </c>
+      <c r="D107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>205</v>
+      </c>
+      <c r="B108" t="s">
+        <v>205</v>
+      </c>
+      <c r="C108" t="s">
+        <v>66</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>206</v>
+      </c>
+      <c r="B109" t="s">
+        <v>206</v>
+      </c>
+      <c r="C109" t="s">
+        <v>207</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>208</v>
+      </c>
+      <c r="B110" t="s">
+        <v>208</v>
+      </c>
+      <c r="C110" t="s">
+        <v>12</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>209</v>
+      </c>
+      <c r="B111" t="s">
+        <v>209</v>
+      </c>
+      <c r="C111" t="s">
+        <v>92</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>0</v>
+      </c>
+      <c r="B112" t="s">
+        <v>210</v>
+      </c>
+      <c r="C112" t="s">
+        <v>211</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>0</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113" t="s">
+        <v>212</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>213</v>
+      </c>
+      <c r="B114" t="s">
+        <v>214</v>
+      </c>
+      <c r="C114" t="s">
+        <v>215</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>216</v>
+      </c>
+      <c r="B115" t="s">
+        <v>216</v>
+      </c>
+      <c r="C115" t="s">
+        <v>10</v>
+      </c>
+      <c r="D115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>217</v>
+      </c>
+      <c r="B116" t="s">
+        <v>217</v>
+      </c>
+      <c r="C116" t="s">
+        <v>84</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>0</v>
+      </c>
+      <c r="B117">
+        <v>0</v>
+      </c>
+      <c r="C117" t="s">
+        <v>212</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>218</v>
+      </c>
+      <c r="B118" t="s">
+        <v>218</v>
+      </c>
+      <c r="C118" t="s">
+        <v>178</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>219</v>
+      </c>
+      <c r="B119" t="s">
+        <v>219</v>
+      </c>
+      <c r="C119" t="s">
+        <v>92</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>220</v>
+      </c>
+      <c r="B120" t="s">
+        <v>220</v>
+      </c>
+      <c r="C120" t="s">
+        <v>221</v>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>222</v>
+      </c>
+      <c r="B121" t="s">
+        <v>222</v>
+      </c>
+      <c r="C121" t="s">
+        <v>16</v>
+      </c>
+      <c r="D121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>223</v>
+      </c>
+      <c r="B122" t="s">
+        <v>223</v>
+      </c>
+      <c r="C122" t="s">
+        <v>224</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>225</v>
+      </c>
+      <c r="B123" t="s">
+        <v>226</v>
+      </c>
+      <c r="C123" t="s">
+        <v>227</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>228</v>
+      </c>
+      <c r="B124" t="s">
+        <v>228</v>
+      </c>
+      <c r="C124" t="s">
+        <v>110</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>229</v>
+      </c>
+      <c r="B125" t="s">
+        <v>229</v>
+      </c>
+      <c r="C125" t="s">
+        <v>230</v>
+      </c>
+      <c r="D125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>231</v>
+      </c>
+      <c r="B126" t="s">
+        <v>231</v>
+      </c>
+      <c r="C126" t="s">
+        <v>232</v>
+      </c>
+      <c r="D126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>233</v>
+      </c>
+      <c r="B127" t="s">
+        <v>233</v>
+      </c>
+      <c r="C127">
+        <v>1</v>
+      </c>
+      <c r="D127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>234</v>
+      </c>
+      <c r="B128" t="s">
+        <v>234</v>
+      </c>
+      <c r="C128" t="s">
+        <v>116</v>
+      </c>
+      <c r="D128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>235</v>
+      </c>
+      <c r="B129" t="s">
+        <v>235</v>
+      </c>
+      <c r="C129" t="s">
+        <v>236</v>
+      </c>
+      <c r="D129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>237</v>
+      </c>
+      <c r="B130" t="s">
+        <v>238</v>
+      </c>
+      <c r="C130" t="s">
+        <v>239</v>
+      </c>
+      <c r="D130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>240</v>
+      </c>
+      <c r="B131" t="s">
+        <v>240</v>
+      </c>
+      <c r="C131" t="s">
+        <v>241</v>
+      </c>
+      <c r="D131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>242</v>
+      </c>
+      <c r="B132" t="s">
+        <v>242</v>
+      </c>
+      <c r="C132" t="s">
+        <v>7</v>
+      </c>
+      <c r="D132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>243</v>
+      </c>
+      <c r="B133" t="s">
+        <v>243</v>
+      </c>
+      <c r="C133" t="s">
+        <v>244</v>
+      </c>
+      <c r="D133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>245</v>
+      </c>
+      <c r="B134" t="s">
+        <v>245</v>
+      </c>
+      <c r="C134" t="s">
+        <v>202</v>
+      </c>
+      <c r="D134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>246</v>
+      </c>
+      <c r="B135" t="s">
+        <v>247</v>
+      </c>
+      <c r="C135" t="s">
+        <v>182</v>
+      </c>
+      <c r="D135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>248</v>
+      </c>
+      <c r="B136" t="s">
+        <v>248</v>
+      </c>
+      <c r="C136" t="s">
+        <v>41</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>249</v>
+      </c>
+      <c r="B137" t="s">
+        <v>250</v>
+      </c>
+      <c r="C137" t="s">
+        <v>251</v>
+      </c>
+      <c r="D137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>252</v>
+      </c>
+      <c r="B138" t="s">
+        <v>253</v>
+      </c>
+      <c r="C138" t="s">
+        <v>10</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>254</v>
+      </c>
+      <c r="B139" t="s">
+        <v>255</v>
+      </c>
+      <c r="C139" t="s">
+        <v>256</v>
+      </c>
+      <c r="D139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>257</v>
+      </c>
+      <c r="B140" t="s">
+        <v>258</v>
+      </c>
+      <c r="C140" t="s">
+        <v>38</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>259</v>
+      </c>
+      <c r="B141" t="s">
+        <v>259</v>
+      </c>
+      <c r="C141" t="s">
+        <v>260</v>
+      </c>
+      <c r="D141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>261</v>
+      </c>
+      <c r="B142" t="s">
+        <v>262</v>
+      </c>
+      <c r="C142" t="s">
+        <v>187</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>263</v>
+      </c>
+      <c r="B143" t="s">
+        <v>264</v>
+      </c>
+      <c r="C143" t="s">
+        <v>265</v>
+      </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>266</v>
+      </c>
+      <c r="B144" t="s">
+        <v>266</v>
+      </c>
+      <c r="C144" t="s">
+        <v>84</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>267</v>
+      </c>
+      <c r="B145" t="s">
+        <v>267</v>
+      </c>
+      <c r="C145" t="s">
+        <v>141</v>
+      </c>
+      <c r="D145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>268</v>
+      </c>
+      <c r="B146" t="s">
+        <v>269</v>
+      </c>
+      <c r="C146" t="s">
+        <v>270</v>
+      </c>
+      <c r="D146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>271</v>
+      </c>
+      <c r="B147" t="s">
+        <v>272</v>
+      </c>
+      <c r="C147" t="s">
+        <v>273</v>
+      </c>
+      <c r="D147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>274</v>
+      </c>
+      <c r="B148" t="s">
+        <v>275</v>
+      </c>
+      <c r="C148" t="s">
+        <v>71</v>
+      </c>
+      <c r="D148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>276</v>
+      </c>
+      <c r="B149" t="s">
+        <v>277</v>
+      </c>
+      <c r="C149" t="s">
+        <v>71</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>278</v>
+      </c>
+      <c r="B150" t="s">
+        <v>279</v>
+      </c>
+      <c r="C150" t="s">
+        <v>110</v>
+      </c>
+      <c r="D150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>280</v>
+      </c>
+      <c r="B151" t="s">
+        <v>281</v>
+      </c>
+      <c r="C151" t="s">
+        <v>236</v>
+      </c>
+      <c r="D151">
         <v>1</v>
       </c>
     </row>

</xml_diff>